<commit_message>
New 30 oct with currencies and bitcoin
30 oct with new currencies without mobility
</commit_message>
<xml_diff>
--- a/Manual/snapshot_graphs.xlsx
+++ b/Manual/snapshot_graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Advait Lath\Documents\nimf-tracker-main\Manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA974590-2EC0-4A40-96E8-DB1CCA6D1923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69BB211-9583-4919-A3CD-F64B694A4286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="0" windowWidth="11844" windowHeight="12240" xr2:uid="{729EB3FA-4BB2-534E-B78E-282A2D9A819C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{729EB3FA-4BB2-534E-B78E-282A2D9A819C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,6 +222,86 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>31 January 2021</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Retail Mobility</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Transit Mobility</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Workplace Mobility</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Grocery Mobility</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Residential Mobility</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.06</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7227-F945-BCA9-AF61B93C1817}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -615,7 +695,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>13-Jul-22</c:v>
+                  <c:v>04-Oct-22</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -639,16 +719,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.7142857142857097E-2</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23428571428571399</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18571428571428497</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45142857142857101</c:v>
+                  <c:v>0.63714285714285701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -671,107 +751,7 @@
         <c:overlap val="-27"/>
         <c:axId val="31241311"/>
         <c:axId val="30967503"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredBarSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>31 January 2021</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:invertIfNegative val="0"/>
-                <c:cat>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$1:$F$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="5"/>
-                      <c:pt idx="0">
-                        <c:v>Retail Mobility</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>Transit Mobility</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>Workplace Mobility</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>Grocery Mobility</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>Residential Mobility</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:cat>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$B$2:$F$2</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0%</c:formatCode>
-                      <c:ptCount val="5"/>
-                      <c:pt idx="0">
-                        <c:v>-0.32</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>-0.14000000000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>-0.09</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>-0.05</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.06</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-7227-F945-BCA9-AF61B93C1817}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredBarSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:barChart>
       <c:catAx>
         <c:axId val="31241311"/>
@@ -1848,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759904DE-AEA7-D24F-B06C-CD1A3C0BFC8A}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:F8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2048,46 +2028,34 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>44755</v>
+        <v>44838</v>
       </c>
       <c r="B8" s="8">
-        <f>4.71428571428571/(100)</f>
-        <v>4.7142857142857097E-2</v>
+        <f>21/(100)</f>
+        <v>0.21</v>
       </c>
       <c r="C8" s="8">
-        <f>23.4285714285714/(100)</f>
-        <v>0.23428571428571399</v>
+        <f>32/(100)</f>
+        <v>0.32</v>
       </c>
       <c r="D8" s="8">
-        <f>18.5714285714285/(100)</f>
-        <v>0.18571428571428497</v>
+        <f>25/(100)</f>
+        <v>0.25</v>
       </c>
       <c r="E8" s="8">
-        <f>45.1428571428571/(100)</f>
-        <v>0.45142857142857101</v>
+        <f>63.7142857142857/(100)</f>
+        <v>0.63714285714285701</v>
       </c>
       <c r="F8" s="8">
-        <f>12.7142857142857/(100)</f>
-        <v>0.127142857142857</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+        <f>11/(100)</f>
+        <v>0.11</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>